<commit_message>
read in data from the workbooks
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_All My Stuff\Senior Year\Algorithms\Project\algorithms_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7075277A-336A-4E81-BD81-F45272AD22CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA4F560-95A8-4745-A02B-D10A15149E46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6890" yWindow="13200" windowWidth="14400" windowHeight="7670" activeTab="1" xr2:uid="{36A8888B-E34B-4134-A916-AA0D47BA0190}"/>
+    <workbookView xWindow="-3700" yWindow="7360" windowWidth="14400" windowHeight="7670" xr2:uid="{36A8888B-E34B-4134-A916-AA0D47BA0190}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -57,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="35">
   <si>
     <t>Sorted by POS</t>
   </si>
@@ -403,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -599,13 +598,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD56DDD-8127-410A-A1D4-6813F110275A}">
   <dimension ref="A1:AR92"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:I65"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8767,1694 +8759,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2347F29-16C2-4363-92D1-0A0F5F31F295}">
-  <dimension ref="A1:H63"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="81" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="81" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="81" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="81" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="81" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="81" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="12">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="81">
-        <v>25</v>
-      </c>
-      <c r="C2" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="82">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E2" s="82">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="F2" s="82">
-        <v>2.4</v>
-      </c>
-      <c r="G2" s="82">
-        <v>0.1</v>
-      </c>
-      <c r="H2" s="82">
-        <v>15.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="12">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="81">
-        <v>31</v>
-      </c>
-      <c r="C3" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="82">
-        <v>5</v>
-      </c>
-      <c r="E3" s="82">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="F3" s="82">
-        <v>2</v>
-      </c>
-      <c r="G3" s="82">
-        <v>0.1</v>
-      </c>
-      <c r="H3" s="82">
-        <v>18.100000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="12">
-        <f t="shared" ref="A4:A61" si="0">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="81">
-        <v>33</v>
-      </c>
-      <c r="C4" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="82">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E4" s="82">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="F4" s="82">
-        <v>2</v>
-      </c>
-      <c r="G4" s="82">
-        <v>0.3</v>
-      </c>
-      <c r="H4" s="82">
-        <v>15.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="12">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="81">
-        <v>34</v>
-      </c>
-      <c r="C5" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="82">
-        <v>5</v>
-      </c>
-      <c r="E5" s="82">
-        <v>6.7</v>
-      </c>
-      <c r="F5" s="82">
-        <v>1.6</v>
-      </c>
-      <c r="G5" s="82">
-        <v>0.2</v>
-      </c>
-      <c r="H5" s="82">
-        <v>17.600000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="12">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="81">
-        <v>24</v>
-      </c>
-      <c r="C6" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="82">
-        <v>5.2</v>
-      </c>
-      <c r="E6" s="82">
-        <v>7.6</v>
-      </c>
-      <c r="F6" s="82">
-        <v>1</v>
-      </c>
-      <c r="G6" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="H6" s="82">
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="12">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="81">
-        <v>24</v>
-      </c>
-      <c r="C7" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="83">
-        <v>2.6</v>
-      </c>
-      <c r="E7" s="83">
-        <v>2.5</v>
-      </c>
-      <c r="F7" s="83">
-        <v>0.9</v>
-      </c>
-      <c r="G7" s="83">
-        <v>0.3</v>
-      </c>
-      <c r="H7" s="83">
-        <v>11.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="12">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="81">
-        <v>27</v>
-      </c>
-      <c r="C8" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="82">
-        <v>2.7</v>
-      </c>
-      <c r="E8" s="82">
-        <v>5.9</v>
-      </c>
-      <c r="F8" s="82">
-        <v>1.2</v>
-      </c>
-      <c r="G8" s="82">
-        <v>0.3</v>
-      </c>
-      <c r="H8" s="82">
-        <v>15.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="12">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="81">
-        <v>28</v>
-      </c>
-      <c r="C9" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="82">
-        <v>4</v>
-      </c>
-      <c r="E9" s="82">
-        <v>7.8</v>
-      </c>
-      <c r="F9" s="82">
-        <v>1.2</v>
-      </c>
-      <c r="G9" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="H9" s="82">
-        <v>15.3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="12">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="81">
-        <v>28</v>
-      </c>
-      <c r="C10" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="82">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E10" s="82">
-        <v>5.9</v>
-      </c>
-      <c r="F10" s="82">
-        <v>1.2</v>
-      </c>
-      <c r="G10" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="H10" s="82">
-        <v>25.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="12">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="81">
-        <v>24</v>
-      </c>
-      <c r="C11" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="82">
-        <v>3.2</v>
-      </c>
-      <c r="E11" s="82">
-        <v>5.8</v>
-      </c>
-      <c r="F11" s="82">
-        <v>1.2</v>
-      </c>
-      <c r="G11" s="82">
-        <v>0.3</v>
-      </c>
-      <c r="H11" s="82">
-        <v>25.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="12">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="81">
-        <v>26</v>
-      </c>
-      <c r="C12" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="82">
-        <v>5</v>
-      </c>
-      <c r="E12" s="82">
-        <v>6.9</v>
-      </c>
-      <c r="F12" s="82">
-        <v>1.5</v>
-      </c>
-      <c r="G12" s="82">
-        <v>0.5</v>
-      </c>
-      <c r="H12" s="82">
-        <v>23.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="12">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="81">
-        <v>23</v>
-      </c>
-      <c r="C13" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="82">
-        <v>3.3</v>
-      </c>
-      <c r="E13" s="82">
-        <v>2.5</v>
-      </c>
-      <c r="F13" s="82">
-        <v>1.2</v>
-      </c>
-      <c r="G13" s="82">
-        <v>0.2</v>
-      </c>
-      <c r="H13" s="82">
-        <v>13.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="12">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="81">
-        <v>30</v>
-      </c>
-      <c r="C14" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="82">
-        <v>3.6</v>
-      </c>
-      <c r="E14" s="82">
-        <v>1.6</v>
-      </c>
-      <c r="F14" s="82">
-        <v>0.9</v>
-      </c>
-      <c r="G14" s="82">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H14" s="82">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="12">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="81">
-        <v>31</v>
-      </c>
-      <c r="C15" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="82">
-        <v>4</v>
-      </c>
-      <c r="E15" s="82">
-        <v>1.6</v>
-      </c>
-      <c r="F15" s="82">
-        <v>0.9</v>
-      </c>
-      <c r="G15" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="H15" s="82">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="12">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" s="81">
-        <v>32</v>
-      </c>
-      <c r="C16" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="82">
-        <v>3.3</v>
-      </c>
-      <c r="E16" s="82">
-        <v>1.3</v>
-      </c>
-      <c r="F16" s="82">
-        <v>1.3</v>
-      </c>
-      <c r="G16" s="82">
-        <v>0.5</v>
-      </c>
-      <c r="H16" s="82">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="12">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="81">
-        <v>26</v>
-      </c>
-      <c r="C17" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="82">
-        <v>4.5</v>
-      </c>
-      <c r="E17" s="82">
-        <v>3.2</v>
-      </c>
-      <c r="F17" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="G17" s="82">
-        <v>0.2</v>
-      </c>
-      <c r="H17" s="82">
-        <v>15.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="12">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="81">
-        <v>32</v>
-      </c>
-      <c r="C18" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="82">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E18" s="82">
-        <v>1.4</v>
-      </c>
-      <c r="F18" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="G18" s="82">
-        <v>0.2</v>
-      </c>
-      <c r="H18" s="82">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="12">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="81">
-        <v>34</v>
-      </c>
-      <c r="C19" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="82">
-        <v>2.4</v>
-      </c>
-      <c r="E19" s="82">
-        <v>2.7</v>
-      </c>
-      <c r="F19" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="G19" s="82">
-        <v>0.2</v>
-      </c>
-      <c r="H19" s="82">
-        <v>18.100000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="12">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="81">
-        <v>20</v>
-      </c>
-      <c r="C20" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="82">
-        <v>2</v>
-      </c>
-      <c r="E20" s="82">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F20" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="G20" s="82">
-        <v>0.1</v>
-      </c>
-      <c r="H20" s="82">
-        <v>7.7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="12">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="81">
-        <v>25</v>
-      </c>
-      <c r="C21" s="81" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="82">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E21" s="82">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F21" s="82">
-        <v>1.2</v>
-      </c>
-      <c r="G21" s="82">
-        <v>0.2</v>
-      </c>
-      <c r="H21" s="82">
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="12">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="81">
-        <v>25</v>
-      </c>
-      <c r="C22" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="82">
-        <v>7.3</v>
-      </c>
-      <c r="E22" s="82">
-        <v>8.6</v>
-      </c>
-      <c r="F22" s="82">
-        <v>1.6</v>
-      </c>
-      <c r="G22" s="82">
-        <v>1</v>
-      </c>
-      <c r="H22" s="82">
-        <v>29.7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="12">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="81">
-        <v>27</v>
-      </c>
-      <c r="C23" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="82">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E23" s="82">
-        <v>5</v>
-      </c>
-      <c r="F23" s="82">
-        <v>1</v>
-      </c>
-      <c r="G23" s="82">
-        <v>1.2</v>
-      </c>
-      <c r="H23" s="82">
-        <v>28.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="12">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="81">
-        <v>24</v>
-      </c>
-      <c r="C24" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="82">
-        <v>5.4</v>
-      </c>
-      <c r="E24" s="82">
-        <v>2.7</v>
-      </c>
-      <c r="F24" s="82">
-        <v>1.6</v>
-      </c>
-      <c r="G24" s="82">
-        <v>0.8</v>
-      </c>
-      <c r="H24" s="82">
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="12">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="81">
-        <v>23</v>
-      </c>
-      <c r="C25" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="82">
-        <v>4.3</v>
-      </c>
-      <c r="E25" s="82">
-        <v>1.8</v>
-      </c>
-      <c r="F25" s="82">
-        <v>1.7</v>
-      </c>
-      <c r="G25" s="82">
-        <v>0.3</v>
-      </c>
-      <c r="H25" s="82">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="12">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="81">
-        <v>24</v>
-      </c>
-      <c r="C26" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="82">
-        <v>5.6</v>
-      </c>
-      <c r="E26" s="82">
-        <v>3.8</v>
-      </c>
-      <c r="F26" s="82">
-        <v>1.8</v>
-      </c>
-      <c r="G26" s="82">
-        <v>0.6</v>
-      </c>
-      <c r="H26" s="82">
-        <v>14.9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="12">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="81">
-        <v>26</v>
-      </c>
-      <c r="C27" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="82">
-        <v>5.2</v>
-      </c>
-      <c r="E27" s="82">
-        <v>3.3</v>
-      </c>
-      <c r="F27" s="82">
-        <v>1.7</v>
-      </c>
-      <c r="G27" s="82">
-        <v>0.6</v>
-      </c>
-      <c r="H27" s="82">
-        <v>10.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="12">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="81">
-        <v>28</v>
-      </c>
-      <c r="C28" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="82">
-        <v>6.2</v>
-      </c>
-      <c r="E28" s="82">
-        <v>2.5</v>
-      </c>
-      <c r="F28" s="82">
-        <v>1.6</v>
-      </c>
-      <c r="G28" s="82">
-        <v>0.3</v>
-      </c>
-      <c r="H28" s="82">
-        <v>14.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="12">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="81">
-        <v>26</v>
-      </c>
-      <c r="C29" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="82">
-        <v>6.6</v>
-      </c>
-      <c r="E29" s="82">
-        <v>3.3</v>
-      </c>
-      <c r="F29" s="82">
-        <v>1.6</v>
-      </c>
-      <c r="G29" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="H29" s="82">
-        <v>23.7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="12">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" s="81">
-        <v>28</v>
-      </c>
-      <c r="C30" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="82">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E30" s="82">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F30" s="82">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G30" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="H30" s="82">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="12">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="81">
-        <v>29</v>
-      </c>
-      <c r="C31" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="82">
-        <v>6.7</v>
-      </c>
-      <c r="E31" s="82">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F31" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="G31" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="H31" s="82">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="12">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="81">
-        <v>26</v>
-      </c>
-      <c r="C32" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="82">
-        <v>5.7</v>
-      </c>
-      <c r="E32" s="82">
-        <v>3.4</v>
-      </c>
-      <c r="F32" s="82">
-        <v>1.8</v>
-      </c>
-      <c r="G32" s="82">
-        <v>0.8</v>
-      </c>
-      <c r="H32" s="82">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="12">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="81">
-        <v>27</v>
-      </c>
-      <c r="C33" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="82">
-        <v>7.3</v>
-      </c>
-      <c r="E33" s="82">
-        <v>3.3</v>
-      </c>
-      <c r="F33" s="82">
-        <v>1.8</v>
-      </c>
-      <c r="G33" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="H33" s="82">
-        <v>26.6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="12">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B34" s="81">
-        <v>29</v>
-      </c>
-      <c r="C34" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" s="82">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E34" s="82">
-        <v>2</v>
-      </c>
-      <c r="F34" s="82">
-        <v>0.9</v>
-      </c>
-      <c r="G34" s="82">
-        <v>0</v>
-      </c>
-      <c r="H34" s="82">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="12">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B35" s="81">
-        <v>27</v>
-      </c>
-      <c r="C35" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="82">
-        <v>6.2</v>
-      </c>
-      <c r="E35" s="82">
-        <v>5.5</v>
-      </c>
-      <c r="F35" s="82">
-        <v>1.9</v>
-      </c>
-      <c r="G35" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="H35" s="82">
-        <v>23.9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="12">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="B36" s="81">
-        <v>29</v>
-      </c>
-      <c r="C36" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" s="82">
-        <v>5.3</v>
-      </c>
-      <c r="E36" s="82">
-        <v>4</v>
-      </c>
-      <c r="F36" s="82">
-        <v>1.8</v>
-      </c>
-      <c r="G36" s="82">
-        <v>0.5</v>
-      </c>
-      <c r="H36" s="82">
-        <v>18.2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="12">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B37" s="81">
-        <v>28</v>
-      </c>
-      <c r="C37" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="82">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E37" s="82">
-        <v>2.5</v>
-      </c>
-      <c r="F37" s="82">
-        <v>1</v>
-      </c>
-      <c r="G37" s="82">
-        <v>0.1</v>
-      </c>
-      <c r="H37" s="82">
-        <v>14.3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="12">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B38" s="81">
-        <v>30</v>
-      </c>
-      <c r="C38" s="81" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" s="82">
-        <v>6</v>
-      </c>
-      <c r="E38" s="82">
-        <v>1.9</v>
-      </c>
-      <c r="F38" s="82">
-        <v>1</v>
-      </c>
-      <c r="G38" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="H38" s="82">
-        <v>12.3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="12">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B39" s="81">
-        <v>33</v>
-      </c>
-      <c r="C39" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="82">
-        <v>8.6</v>
-      </c>
-      <c r="E39" s="82">
-        <v>9.1</v>
-      </c>
-      <c r="F39" s="82">
-        <v>9.1</v>
-      </c>
-      <c r="G39" s="82">
-        <v>0.9</v>
-      </c>
-      <c r="H39" s="82">
-        <v>27.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="12">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B40" s="81">
-        <v>24</v>
-      </c>
-      <c r="C40" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="82">
-        <v>5.2</v>
-      </c>
-      <c r="E40" s="82">
-        <v>1</v>
-      </c>
-      <c r="F40" s="82">
-        <v>0.8</v>
-      </c>
-      <c r="G40" s="82">
-        <v>1.3</v>
-      </c>
-      <c r="H40" s="82">
-        <v>13.6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="12">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B41" s="81">
-        <v>25</v>
-      </c>
-      <c r="C41" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="82">
-        <v>3.5</v>
-      </c>
-      <c r="E41" s="82">
-        <v>1.2</v>
-      </c>
-      <c r="F41" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="G41" s="82">
-        <v>0.8</v>
-      </c>
-      <c r="H41" s="82">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="12">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B42" s="81">
-        <v>23</v>
-      </c>
-      <c r="C42" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="82">
-        <v>8</v>
-      </c>
-      <c r="E42" s="82">
-        <v>2.6</v>
-      </c>
-      <c r="F42" s="82">
-        <v>0.5</v>
-      </c>
-      <c r="G42" s="82">
-        <v>0.5</v>
-      </c>
-      <c r="H42" s="82">
-        <v>16.100000000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="12">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B43" s="81">
-        <v>24</v>
-      </c>
-      <c r="C43" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" s="82">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="E43" s="82">
-        <v>3.1</v>
-      </c>
-      <c r="F43" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="G43" s="82">
-        <v>0.6</v>
-      </c>
-      <c r="H43" s="82">
-        <v>21.4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="12">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B44" s="81">
-        <v>29</v>
-      </c>
-      <c r="C44" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="82">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E44" s="82">
-        <v>1.3</v>
-      </c>
-      <c r="F44" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="G44" s="82">
-        <v>0.3</v>
-      </c>
-      <c r="H44" s="82">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="12">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B45" s="81">
-        <v>30</v>
-      </c>
-      <c r="C45" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" s="82">
-        <v>6.1</v>
-      </c>
-      <c r="E45" s="82">
-        <v>2.6</v>
-      </c>
-      <c r="F45" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="G45" s="82">
-        <v>0.3</v>
-      </c>
-      <c r="H45" s="82">
-        <v>19.8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="12">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B46" s="81">
-        <v>31</v>
-      </c>
-      <c r="C46" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" s="82">
-        <v>5.2</v>
-      </c>
-      <c r="E46" s="82">
-        <v>1.9</v>
-      </c>
-      <c r="F46" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="G46" s="82">
-        <v>0.1</v>
-      </c>
-      <c r="H46" s="82">
-        <v>18.7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="12">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B47" s="81">
-        <v>27</v>
-      </c>
-      <c r="C47" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" s="82">
-        <v>9</v>
-      </c>
-      <c r="E47" s="82">
-        <v>1.8</v>
-      </c>
-      <c r="F47" s="82">
-        <v>1.5</v>
-      </c>
-      <c r="G47" s="82">
-        <v>0.5</v>
-      </c>
-      <c r="H47" s="82">
-        <v>15.1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="12">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B48" s="81">
-        <v>30</v>
-      </c>
-      <c r="C48" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D48" s="82">
-        <v>6.5</v>
-      </c>
-      <c r="E48" s="82">
-        <v>2.5</v>
-      </c>
-      <c r="F48" s="82">
-        <v>1.5</v>
-      </c>
-      <c r="G48" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="H48" s="82">
-        <v>12.6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="12">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B49" s="81">
-        <v>24</v>
-      </c>
-      <c r="C49" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D49" s="82">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="E49" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="F49" s="82">
-        <v>0.3</v>
-      </c>
-      <c r="G49" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="H49" s="82">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" s="12">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B50" s="81">
-        <v>25</v>
-      </c>
-      <c r="C50" s="81" t="s">
-        <v>16</v>
-      </c>
-      <c r="D50" s="82">
-        <v>7.6</v>
-      </c>
-      <c r="E50" s="82">
-        <v>1.2</v>
-      </c>
-      <c r="F50" s="82">
-        <v>0.6</v>
-      </c>
-      <c r="G50" s="82">
-        <v>1.2</v>
-      </c>
-      <c r="H50" s="82">
-        <v>8.3000000000000007</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" s="12">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B51" s="81">
-        <v>24</v>
-      </c>
-      <c r="C51" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D51" s="82">
-        <v>7.5</v>
-      </c>
-      <c r="E51" s="82">
-        <v>1.2</v>
-      </c>
-      <c r="F51" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="G51" s="82">
-        <v>0.9</v>
-      </c>
-      <c r="H51" s="82">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" s="12">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B52" s="81">
-        <v>29</v>
-      </c>
-      <c r="C52" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D52" s="82">
-        <v>7.3</v>
-      </c>
-      <c r="E52" s="82">
-        <v>3.2</v>
-      </c>
-      <c r="F52" s="82">
-        <v>0.8</v>
-      </c>
-      <c r="G52" s="82">
-        <v>1.5</v>
-      </c>
-      <c r="H52" s="82">
-        <v>15.2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A53" s="12">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B53" s="81">
-        <v>32</v>
-      </c>
-      <c r="C53" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" s="82">
-        <v>6.7</v>
-      </c>
-      <c r="E53" s="82">
-        <v>4.2</v>
-      </c>
-      <c r="F53" s="82">
-        <v>0.9</v>
-      </c>
-      <c r="G53" s="82">
-        <v>1.3</v>
-      </c>
-      <c r="H53" s="82">
-        <v>13.6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" s="12">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B54" s="81">
-        <v>33</v>
-      </c>
-      <c r="C54" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" s="82">
-        <v>6.8</v>
-      </c>
-      <c r="E54" s="82">
-        <v>4</v>
-      </c>
-      <c r="F54" s="82">
-        <v>0.8</v>
-      </c>
-      <c r="G54" s="82">
-        <v>0.9</v>
-      </c>
-      <c r="H54" s="82">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A55" s="12">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B55" s="81">
-        <v>24</v>
-      </c>
-      <c r="C55" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D55" s="82">
-        <v>6.7</v>
-      </c>
-      <c r="E55" s="82">
-        <v>0.9</v>
-      </c>
-      <c r="F55" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="G55" s="82">
-        <v>0.5</v>
-      </c>
-      <c r="H55" s="82">
-        <v>14.3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A56" s="12">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B56" s="81">
-        <v>27</v>
-      </c>
-      <c r="C56" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D56" s="82">
-        <v>7.4</v>
-      </c>
-      <c r="E56" s="82">
-        <v>1</v>
-      </c>
-      <c r="F56" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="G56" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="H56" s="82">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A57" s="12">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B57" s="81">
-        <v>33</v>
-      </c>
-      <c r="C57" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D57" s="82">
-        <v>6.4</v>
-      </c>
-      <c r="E57" s="82">
-        <v>1.2</v>
-      </c>
-      <c r="F57" s="82">
-        <v>0.8</v>
-      </c>
-      <c r="G57" s="82">
-        <v>0.6</v>
-      </c>
-      <c r="H57" s="82">
-        <v>10.8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A58" s="12">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B58" s="81">
-        <v>28</v>
-      </c>
-      <c r="C58" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D58" s="82">
-        <v>7.4</v>
-      </c>
-      <c r="E58" s="82">
-        <v>0.5</v>
-      </c>
-      <c r="F58" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="G58" s="82">
-        <v>0.7</v>
-      </c>
-      <c r="H58" s="82">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A59" s="12">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B59" s="81">
-        <v>29</v>
-      </c>
-      <c r="C59" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D59" s="82">
-        <v>8.6</v>
-      </c>
-      <c r="E59" s="82">
-        <v>0.8</v>
-      </c>
-      <c r="F59" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="G59" s="82">
-        <v>0.4</v>
-      </c>
-      <c r="H59" s="82">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A60" s="12">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B60" s="81">
-        <v>26</v>
-      </c>
-      <c r="C60" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60" s="82">
-        <v>14.5</v>
-      </c>
-      <c r="E60" s="82">
-        <v>1.9</v>
-      </c>
-      <c r="F60" s="82">
-        <v>1.5</v>
-      </c>
-      <c r="G60" s="82">
-        <v>2.1</v>
-      </c>
-      <c r="H60" s="82">
-        <v>20.6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A61" s="12">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B61" s="81">
-        <v>27</v>
-      </c>
-      <c r="C61" s="81" t="s">
-        <v>18</v>
-      </c>
-      <c r="D61" s="82">
-        <v>12.4</v>
-      </c>
-      <c r="E61" s="82">
-        <v>1.4</v>
-      </c>
-      <c r="F61" s="82">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G61" s="82">
-        <v>2.4</v>
-      </c>
-      <c r="H61" s="82">
-        <v>17.100000000000001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A62" s="12"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="82"/>
-      <c r="E62" s="82"/>
-      <c r="F62" s="82"/>
-      <c r="G62" s="82"/>
-      <c r="H62" s="82"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A63" s="12"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="82"/>
-      <c r="E63" s="82"/>
-      <c r="F63" s="82"/>
-      <c r="G63" s="82"/>
-      <c r="H63" s="82"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10643,15 +8951,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{918FAEA0-A5F6-4F87-B713-41F1A01C70D0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34B6824B-EDD0-411D-84FA-DCF3EFA40CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10676,10 +8988,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34B6824B-EDD0-411D-84FA-DCF3EFA40CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{918FAEA0-A5F6-4F87-B713-41F1A01C70D0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>